<commit_message>
small change to the excel file
</commit_message>
<xml_diff>
--- a/digipalvelut-projekti/static/impact_tool.xlsx
+++ b/digipalvelut-projekti/static/impact_tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gr289361\Desktop\projekti\digipalvelut-projekti\digipalvelut-projekti\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E323AC59-EB96-4241-A756-728DEE783039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA6E110-0DF0-485F-8247-23EA352F57ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="1010" windowWidth="14400" windowHeight="7280" xr2:uid="{D048ECE2-60FA-4AD2-9F24-90A95A17B271}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{D048ECE2-60FA-4AD2-9F24-90A95A17B271}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Target</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>End</t>
-  </si>
-  <si>
-    <t>Percent</t>
   </si>
   <si>
     <t>Unit</t>
@@ -455,7 +452,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -470,7 +467,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -484,9 +481,7 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -732,20 +727,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -768,14 +763,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AB3B2CB-9EE9-4AC4-9E93-74508007D977}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -790,4 +777,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>